<commit_message>
[FIX]pabi_budget_xls: added formula for total budget ref: issues/1186 point-3
</commit_message>
<xml_diff>
--- a/pabi_budget_xls/template/Template_Section_Plan.xlsx
+++ b/pabi_budget_xls/template/Template_Section_Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="708" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="708" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Section" sheetId="1" state="visible" r:id="rId2"/>
@@ -1511,7 +1511,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1552,15 +1552,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1650,6 +1650,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1804,7 +1808,7 @@
   <dimension ref="A2:I56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2306,8 +2310,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2335,7 +2339,7 @@
   <dimension ref="A2:B41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2427,7 +2431,7 @@
   <dimension ref="A2:B32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2704,8 +2708,8 @@
   </sheetPr>
   <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5825,7 +5829,7 @@
       <c r="A4" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>157</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -6857,7 +6861,7 @@
       <c r="A5" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>159</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -7889,7 +7893,7 @@
       <c r="A6" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>161</v>
       </c>
       <c r="C6" s="13"/>
@@ -12137,7 +12141,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12169,7 +12173,7 @@
       <c r="A1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="10" t="n">
+      <c r="B1" s="35" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -12177,7 +12181,7 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -12185,7 +12189,7 @@
       <c r="A3" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <v>105064</v>
       </c>
     </row>
@@ -12193,7 +12197,7 @@
       <c r="A4" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>200</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -12201,64 +12205,64 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-    </row>
-    <row r="8" s="42" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+    </row>
+    <row r="8" s="43" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="24" t="s">
         <v>181</v>
       </c>
@@ -12271,370 +12275,370 @@
       <c r="H9" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="P9" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="S9" s="41" t="s">
+      <c r="S9" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="T9" s="41" t="s">
+      <c r="T9" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="U9" s="41" t="s">
+      <c r="U9" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="V9" s="41" t="s">
+      <c r="V9" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="W9" s="41" t="s">
+      <c r="W9" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="X9" s="41" t="s">
+      <c r="X9" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="Y9" s="41" t="s">
+      <c r="Y9" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="Z9" s="41" t="s">
+      <c r="Z9" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="AA9" s="41" t="s">
+      <c r="AA9" s="42" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="45" t="n">
+      <c r="E10" s="46" t="n">
         <v>12</v>
       </c>
-      <c r="F10" s="46" t="n">
+      <c r="F10" s="47" t="n">
         <v>10000</v>
       </c>
-      <c r="G10" s="45" t="n">
+      <c r="G10" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="47" t="n">
+      <c r="H10" s="48" t="n">
         <f aca="false">E10*F10*G10</f>
         <v>120000</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46" t="n">
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47" t="n">
         <f aca="false">H10</f>
         <v>120000</v>
       </c>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="48" t="n">
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="49" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>120000</v>
       </c>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="49" t="n">
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="50" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>120000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="45" t="n">
+      <c r="E11" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="46" t="n">
+      <c r="F11" s="47" t="n">
         <v>10000</v>
       </c>
-      <c r="G11" s="45" t="n">
+      <c r="G11" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="47" t="n">
+      <c r="H11" s="48" t="n">
         <f aca="false">E11*F11*G11</f>
         <v>30000</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46" t="n">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47" t="n">
         <f aca="false">H11</f>
         <v>30000</v>
       </c>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="48" t="n">
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="49" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>30000</v>
       </c>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="49" t="n">
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="50" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>30000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="45" t="n">
+      <c r="E12" s="46" t="n">
         <v>50</v>
       </c>
-      <c r="F12" s="46" t="n">
+      <c r="F12" s="47" t="n">
         <v>300</v>
       </c>
-      <c r="G12" s="45" t="n">
+      <c r="G12" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="47" t="n">
+      <c r="H12" s="48" t="n">
         <f aca="false">E12*F12*G12</f>
         <v>15000</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46" t="n">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47" t="n">
         <f aca="false">H12</f>
         <v>15000</v>
       </c>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="48" t="n">
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="49" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>15000</v>
       </c>
-      <c r="W12" s="46"/>
-      <c r="X12" s="46"/>
-      <c r="Y12" s="46"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="49" t="n">
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="50" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>15000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="46" t="n">
+      <c r="F13" s="47" t="n">
         <v>500</v>
       </c>
-      <c r="G13" s="45" t="n">
+      <c r="G13" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="47" t="n">
+      <c r="H13" s="48" t="n">
         <f aca="false">E13*F13*G13</f>
         <v>1500</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46" t="n">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47" t="n">
         <f aca="false">H13</f>
         <v>1500</v>
       </c>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="48" t="n">
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="49" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>1500</v>
       </c>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="49" t="n">
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="50" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>1500</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="G14" s="52" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="G14" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="H14" s="47" t="n">
+      <c r="H14" s="48" t="n">
         <f aca="false">SUM(H10:H13)</f>
         <v>166500</v>
       </c>
-      <c r="I14" s="46" t="n">
+      <c r="I14" s="47" t="n">
         <f aca="false">SUM(I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="46" t="n">
+      <c r="J14" s="47" t="n">
         <f aca="false">SUM(J10:J13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="46" t="n">
+      <c r="K14" s="47" t="n">
         <f aca="false">SUM(K10:K13)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="46" t="n">
+      <c r="L14" s="47" t="n">
         <f aca="false">SUM(L10:L13)</f>
         <v>166500</v>
       </c>
-      <c r="M14" s="46" t="n">
+      <c r="M14" s="47" t="n">
         <f aca="false">SUM(M10:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="46" t="n">
+      <c r="N14" s="47" t="n">
         <f aca="false">SUM(N10:N13)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="46" t="n">
+      <c r="O14" s="47" t="n">
         <f aca="false">SUM(O10:O13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="46" t="n">
+      <c r="P14" s="47" t="n">
         <f aca="false">SUM(P10:P13)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="46" t="n">
+      <c r="Q14" s="47" t="n">
         <f aca="false">SUM(Q10:Q13)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="46" t="n">
+      <c r="R14" s="47" t="n">
         <f aca="false">SUM(R10:R13)</f>
         <v>0</v>
       </c>
-      <c r="S14" s="46" t="n">
+      <c r="S14" s="47" t="n">
         <f aca="false">SUM(S10:S13)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="46" t="n">
+      <c r="T14" s="47" t="n">
         <f aca="false">SUM(T10:T13)</f>
         <v>0</v>
       </c>
-      <c r="U14" s="46" t="n">
+      <c r="U14" s="47" t="n">
         <f aca="false">SUM(U10:U13)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="48" t="n">
+      <c r="V14" s="49" t="n">
         <f aca="false">SUM(J14:U14)</f>
         <v>166500</v>
       </c>
-      <c r="W14" s="46" t="n">
+      <c r="W14" s="47" t="n">
         <f aca="false">SUM(W10:W13)</f>
         <v>0</v>
       </c>
-      <c r="X14" s="46" t="n">
+      <c r="X14" s="47" t="n">
         <f aca="false">SUM(X10:X13)</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="46" t="n">
+      <c r="Y14" s="47" t="n">
         <f aca="false">SUM(Y10:Y13)</f>
         <v>0</v>
       </c>
-      <c r="Z14" s="46" t="n">
+      <c r="Z14" s="47" t="n">
         <f aca="false">SUM(Z10:Z13)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="49" t="n">
+      <c r="AA14" s="50" t="n">
         <f aca="false">SUM(AA10:AA13)</f>
         <v>166500</v>
       </c>
@@ -12664,7 +12668,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12687,7 +12691,7 @@
       <c r="A1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="10" t="n">
+      <c r="B1" s="35" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -12695,7 +12699,7 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -12703,7 +12707,7 @@
       <c r="A3" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <v>105064</v>
       </c>
     </row>
@@ -12711,7 +12715,7 @@
       <c r="A4" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>212</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -12719,64 +12723,64 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-    </row>
-    <row r="8" s="42" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+    </row>
+    <row r="8" s="43" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="24" t="s">
         <v>181</v>
       </c>
@@ -12789,370 +12793,370 @@
       <c r="H9" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="P9" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="S9" s="41" t="s">
+      <c r="S9" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="T9" s="41" t="s">
+      <c r="T9" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="U9" s="41" t="s">
+      <c r="U9" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="V9" s="41" t="s">
+      <c r="V9" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="W9" s="41" t="s">
+      <c r="W9" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="X9" s="41" t="s">
+      <c r="X9" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="Y9" s="41" t="s">
+      <c r="Y9" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="Z9" s="41" t="s">
+      <c r="Z9" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="AA9" s="41" t="s">
+      <c r="AA9" s="42" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="45" t="n">
+      <c r="E10" s="46" t="n">
         <v>12</v>
       </c>
-      <c r="F10" s="46" t="n">
+      <c r="F10" s="47" t="n">
         <v>10000</v>
       </c>
-      <c r="G10" s="45" t="n">
+      <c r="G10" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="47" t="n">
+      <c r="H10" s="48" t="n">
         <f aca="false">E10*F10*G10</f>
         <v>120000</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46" t="n">
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47" t="n">
         <f aca="false">H10</f>
         <v>120000</v>
       </c>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="48" t="n">
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="49" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>120000</v>
       </c>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="49" t="n">
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="50" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>120000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E11" s="45" t="n">
+      <c r="E11" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="F11" s="46" t="n">
+      <c r="F11" s="47" t="n">
         <v>10000</v>
       </c>
-      <c r="G11" s="45" t="n">
+      <c r="G11" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="47" t="n">
+      <c r="H11" s="48" t="n">
         <f aca="false">E11*F11*G11</f>
         <v>30000</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46" t="n">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47" t="n">
         <f aca="false">H11</f>
         <v>30000</v>
       </c>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="48" t="n">
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="49" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>30000</v>
       </c>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="49" t="n">
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="50" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>30000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="45" t="n">
+      <c r="E12" s="46" t="n">
         <v>50</v>
       </c>
-      <c r="F12" s="46" t="n">
+      <c r="F12" s="47" t="n">
         <v>300</v>
       </c>
-      <c r="G12" s="45" t="n">
+      <c r="G12" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="47" t="n">
+      <c r="H12" s="48" t="n">
         <f aca="false">E12*F12*G12</f>
         <v>15000</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46" t="n">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47" t="n">
         <f aca="false">H12</f>
         <v>15000</v>
       </c>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="48" t="n">
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="49" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>15000</v>
       </c>
-      <c r="W12" s="46"/>
-      <c r="X12" s="46"/>
-      <c r="Y12" s="46"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="49" t="n">
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="50" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>15000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="46" t="n">
+      <c r="F13" s="47" t="n">
         <v>500</v>
       </c>
-      <c r="G13" s="45" t="n">
+      <c r="G13" s="46" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="47" t="n">
+      <c r="H13" s="48" t="n">
         <f aca="false">E13*F13*G13</f>
         <v>1500</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46" t="n">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47" t="n">
         <f aca="false">H13</f>
         <v>1500</v>
       </c>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="48" t="n">
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="49" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>1500</v>
       </c>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="49" t="n">
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="50" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>1500</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="G14" s="52" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="G14" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="H14" s="47" t="n">
+      <c r="H14" s="48" t="n">
         <f aca="false">SUM(H10:H13)</f>
         <v>166500</v>
       </c>
-      <c r="I14" s="46" t="n">
+      <c r="I14" s="47" t="n">
         <f aca="false">SUM(I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="46" t="n">
+      <c r="J14" s="47" t="n">
         <f aca="false">SUM(J10:J13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="46" t="n">
+      <c r="K14" s="47" t="n">
         <f aca="false">SUM(K10:K13)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="46" t="n">
+      <c r="L14" s="47" t="n">
         <f aca="false">SUM(L10:L13)</f>
         <v>166500</v>
       </c>
-      <c r="M14" s="46" t="n">
+      <c r="M14" s="47" t="n">
         <f aca="false">SUM(M10:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="46" t="n">
+      <c r="N14" s="47" t="n">
         <f aca="false">SUM(N10:N13)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="46" t="n">
+      <c r="O14" s="47" t="n">
         <f aca="false">SUM(O10:O13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="46" t="n">
+      <c r="P14" s="47" t="n">
         <f aca="false">SUM(P10:P13)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="46" t="n">
+      <c r="Q14" s="47" t="n">
         <f aca="false">SUM(Q10:Q13)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="46" t="n">
+      <c r="R14" s="47" t="n">
         <f aca="false">SUM(R10:R13)</f>
         <v>0</v>
       </c>
-      <c r="S14" s="46" t="n">
+      <c r="S14" s="47" t="n">
         <f aca="false">SUM(S10:S13)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="46" t="n">
+      <c r="T14" s="47" t="n">
         <f aca="false">SUM(T10:T13)</f>
         <v>0</v>
       </c>
-      <c r="U14" s="46" t="n">
+      <c r="U14" s="47" t="n">
         <f aca="false">SUM(U10:U13)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="48" t="n">
+      <c r="V14" s="49" t="n">
         <f aca="false">SUM(J14:U14)</f>
         <v>166500</v>
       </c>
-      <c r="W14" s="46" t="n">
+      <c r="W14" s="47" t="n">
         <f aca="false">SUM(W10:W13)</f>
         <v>0</v>
       </c>
-      <c r="X14" s="46" t="n">
+      <c r="X14" s="47" t="n">
         <f aca="false">SUM(X10:X13)</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="46" t="n">
+      <c r="Y14" s="47" t="n">
         <f aca="false">SUM(Y10:Y13)</f>
         <v>0</v>
       </c>
-      <c r="Z14" s="46" t="n">
+      <c r="Z14" s="47" t="n">
         <f aca="false">SUM(Z10:Z13)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="49" t="n">
+      <c r="AA14" s="50" t="n">
         <f aca="false">SUM(AA10:AA13)</f>
         <v>166500</v>
       </c>
@@ -13182,7 +13186,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -13205,7 +13209,7 @@
       <c r="A1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="10" t="n">
+      <c r="B1" s="35" t="n">
         <v>2016</v>
       </c>
     </row>
@@ -13213,7 +13217,7 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -13221,7 +13225,7 @@
       <c r="A3" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <v>105064</v>
       </c>
     </row>
@@ -13229,7 +13233,7 @@
       <c r="A4" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>213</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -13237,64 +13241,64 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-    </row>
-    <row r="8" s="42" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+    </row>
+    <row r="8" s="43" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="42"/>
+      <c r="Z8" s="42"/>
+      <c r="AA8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="24" t="s">
         <v>181</v>
       </c>
@@ -13307,314 +13311,314 @@
       <c r="H9" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="L9" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="P9" s="41" t="s">
+      <c r="P9" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="S9" s="41" t="s">
+      <c r="S9" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="T9" s="41" t="s">
+      <c r="T9" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="U9" s="41" t="s">
+      <c r="U9" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="V9" s="41" t="s">
+      <c r="V9" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="W9" s="41" t="s">
+      <c r="W9" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="X9" s="41" t="s">
+      <c r="X9" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="Y9" s="41" t="s">
+      <c r="Y9" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="Z9" s="41" t="s">
+      <c r="Z9" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="AA9" s="41" t="s">
+      <c r="AA9" s="42" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="47" t="n">
+      <c r="A10" s="45"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="48" t="n">
         <f aca="false">E10*F10*G10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46" t="n">
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47" t="n">
         <f aca="false">H10</f>
         <v>0</v>
       </c>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="46"/>
-      <c r="R10" s="46"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="48" t="n">
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="49" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>0</v>
       </c>
-      <c r="W10" s="46"/>
-      <c r="X10" s="46"/>
-      <c r="Y10" s="46"/>
-      <c r="Z10" s="46"/>
-      <c r="AA10" s="49" t="n">
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="50" t="n">
         <f aca="false">SUM(I10:U10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="44"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="47" t="n">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="48" t="n">
         <f aca="false">E11*F11*G11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46" t="n">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47" t="n">
         <f aca="false">H11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="48" t="n">
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="49" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>0</v>
       </c>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="46"/>
-      <c r="AA11" s="49" t="n">
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="50" t="n">
         <f aca="false">SUM(I11:U11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="47" t="n">
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="48" t="n">
         <f aca="false">E12*F12*G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46" t="n">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47" t="n">
         <f aca="false">H12</f>
         <v>0</v>
       </c>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="48" t="n">
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="49" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>0</v>
       </c>
-      <c r="W12" s="46"/>
-      <c r="X12" s="46"/>
-      <c r="Y12" s="46"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="49" t="n">
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="50" t="n">
         <f aca="false">SUM(I12:U12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="47" t="n">
+      <c r="A13" s="45"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="48" t="n">
         <f aca="false">E13*F13*G13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46" t="n">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47" t="n">
         <f aca="false">H13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="48" t="n">
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="49" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>0</v>
       </c>
-      <c r="W13" s="46"/>
-      <c r="X13" s="46"/>
-      <c r="Y13" s="46"/>
-      <c r="Z13" s="46"/>
-      <c r="AA13" s="49" t="n">
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="50" t="n">
         <f aca="false">SUM(I13:U13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="G14" s="52" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="G14" s="53" t="s">
         <v>177</v>
       </c>
-      <c r="H14" s="47" t="n">
+      <c r="H14" s="48" t="n">
         <f aca="false">SUM(H10:H13)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="46" t="n">
+      <c r="I14" s="47" t="n">
         <f aca="false">SUM(I10:I13)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="46" t="n">
+      <c r="J14" s="47" t="n">
         <f aca="false">SUM(J10:J13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="46" t="n">
+      <c r="K14" s="47" t="n">
         <f aca="false">SUM(K10:K13)</f>
         <v>0</v>
       </c>
-      <c r="L14" s="46" t="n">
+      <c r="L14" s="47" t="n">
         <f aca="false">SUM(L10:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="46" t="n">
+      <c r="M14" s="47" t="n">
         <f aca="false">SUM(M10:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="46" t="n">
+      <c r="N14" s="47" t="n">
         <f aca="false">SUM(N10:N13)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="46" t="n">
+      <c r="O14" s="47" t="n">
         <f aca="false">SUM(O10:O13)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="46" t="n">
+      <c r="P14" s="47" t="n">
         <f aca="false">SUM(P10:P13)</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="46" t="n">
+      <c r="Q14" s="47" t="n">
         <f aca="false">SUM(Q10:Q13)</f>
         <v>0</v>
       </c>
-      <c r="R14" s="46" t="n">
+      <c r="R14" s="47" t="n">
         <f aca="false">SUM(R10:R13)</f>
         <v>0</v>
       </c>
-      <c r="S14" s="46" t="n">
+      <c r="S14" s="47" t="n">
         <f aca="false">SUM(S10:S13)</f>
         <v>0</v>
       </c>
-      <c r="T14" s="46" t="n">
+      <c r="T14" s="47" t="n">
         <f aca="false">SUM(T10:T13)</f>
         <v>0</v>
       </c>
-      <c r="U14" s="46" t="n">
+      <c r="U14" s="47" t="n">
         <f aca="false">SUM(U10:U13)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="48" t="n">
+      <c r="V14" s="49" t="n">
         <f aca="false">SUM(J14:U14)</f>
         <v>0</v>
       </c>
-      <c r="W14" s="46" t="n">
+      <c r="W14" s="47" t="n">
         <f aca="false">SUM(W10:W13)</f>
         <v>0</v>
       </c>
-      <c r="X14" s="46" t="n">
+      <c r="X14" s="47" t="n">
         <f aca="false">SUM(X10:X13)</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="46" t="n">
+      <c r="Y14" s="47" t="n">
         <f aca="false">SUM(Y10:Y13)</f>
         <v>0</v>
       </c>
-      <c r="Z14" s="46" t="n">
+      <c r="Z14" s="47" t="n">
         <f aca="false">SUM(Z10:Z13)</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="49" t="n">
+      <c r="AA14" s="50" t="n">
         <f aca="false">SUM(AA10:AA13)</f>
         <v>0</v>
       </c>

</xml_diff>